<commit_message>
Actualización menor de ejemplos
Ejemplos actualizados
</commit_message>
<xml_diff>
--- a/Ejs4-i (Figs y Tablas)/figs/EjFigsExcel.xlsx
+++ b/Ejs4-i (Figs y Tablas)/figs/EjFigsExcel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17668"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus.Salido\Documents\Docencia\Asignaturas\LaTeXPress\Ejemplos\Ejemplos-2017\EjsFigsTables\figs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus.Salido\Documents\GitHub\latex\Curso-LaTeX4TFG\Ejs4-i (Figs y Tablas)\figs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AF229A-22B9-4B2A-8FA5-F15099FD0F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="8565" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,6 +142,39 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Implantación de SO</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35234711286089232"/>
+          <c:y val="7.407407407407407E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -153,7 +187,7 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr algn="ctr">
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -1566,7 +1600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1649,11 +1683,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>